<commit_message>
praktikum 2 sbd done and some updates
</commit_message>
<xml_diff>
--- a/Semester 1/EF234101 - Fundamental Programming/Praktikum/praktikum-3/s3.xlsx
+++ b/Semester 1/EF234101 - Fundamental Programming/Praktikum/praktikum-3/s3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itsacid-my.sharepoint.com/personal/5025231014_student_its_ac_id/Documents/Uni-assignments/Semester 1/EF234101 - Fundamental Programming/Praktikum/praktikum-3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Institut Teknologi Sepuluh Nopember\Uni-assignments\Semester 1\EF234101 - Fundamental Programming\Praktikum\praktikum-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7716DE6-B917-4B4E-B4CA-70696D5F66BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACA3315-156D-4797-888E-BB40DDFC8C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{BD865EB0-40E5-4E8A-A7B8-53DB19AD258D}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="52">
   <si>
     <t>.</t>
   </si>
@@ -185,6 +184,15 @@
   </si>
   <si>
     <t>(3, 2)</t>
+  </si>
+  <si>
+    <t>1, 33</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -238,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,9 +267,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -580,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E86C21-E511-484D-9D05-519FB2825A46}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1240,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFB7459-8556-4AD6-BE60-43CAD9F67824}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,13 +1256,13 @@
     <col min="1" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="8.88671875" style="7"/>
     <col min="11" max="11" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.109375" style="1" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1265,7 +1270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1275,11 +1280,11 @@
       <c r="I2" s="1">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1289,11 +1294,11 @@
       <c r="I3" s="1">
         <v>3</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1303,11 +1308,11 @@
       <c r="I4" s="1">
         <v>4</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>1</v>
       </c>
@@ -1330,11 +1335,11 @@
       <c r="I6" s="1">
         <v>3</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -1357,11 +1362,11 @@
       <c r="I7" s="1">
         <v>5</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -1384,11 +1389,11 @@
       <c r="I8" s="1">
         <v>7</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>10</v>
       </c>
@@ -1403,11 +1408,19 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+    <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2">
+        <v>33</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="1" t="s">
         <v>5</v>
@@ -1418,8 +1431,23 @@
       <c r="I10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1429,16 +1457,69 @@
       <c r="I11" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I12" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="1">
+        <v>13</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1451,8 +1532,23 @@
       <c r="D14" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -1466,7 +1562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>6</v>
       </c>
@@ -1740,7 +1836,7 @@
       <c r="D41" s="2">
         <v>7</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F41" s="1">
@@ -1768,23 +1864,19 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
+      <c r="A43" s="2"/>
       <c r="E43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="1">
         <v>16</v>
       </c>
     </row>
@@ -1848,7 +1940,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E49" s="1" t="s">
         <v>36</v>
       </c>
@@ -1856,31 +1948,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7" t="s">
+    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E50" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F50" s="5">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7" t="s">
+    <row r="51" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E51" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F51" s="5">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E52" s="1" t="s">
         <v>39</v>
       </c>
@@ -1888,7 +1972,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1896,7 +1980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E54" s="1" t="s">
         <v>41</v>
       </c>
@@ -1904,7 +1988,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E55" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>